<commit_message>
Fix in lab3 MatProg
</commit_message>
<xml_diff>
--- a/MatProg/Lab3/Lab3.xlsx
+++ b/MatProg/Lab3/Lab3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MatProg\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FB9864-C08E-4F94-A84E-6774C94F7C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D57B8D-13EC-4DFE-871E-B3AC0B29117D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="3240" windowWidth="21600" windowHeight="9540" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Решение без ограничений" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
   <si>
     <t>Условие</t>
   </si>
@@ -774,7 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -816,14 +816,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -832,16 +832,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1333,7 +1326,19 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>1,4</m:t>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>4</m:t>
                             </m:r>
                           </m:e>
                         </m:acc>
@@ -1597,7 +1602,19 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>1,4</m:t>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>4</m:t>
                             </m:r>
                           </m:e>
                         </m:acc>
@@ -6544,7 +6561,19 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>1,4</m:t>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>4</m:t>
                             </m:r>
                           </m:e>
                         </m:acc>
@@ -6803,7 +6832,19 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>1,4</m:t>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>4</m:t>
                             </m:r>
                           </m:e>
                         </m:acc>
@@ -9014,6 +9055,1370 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2914901" cy="495072"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12233F23-6E7E-E5A4-224B-8A8A6A608589}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7305675" y="4414837"/>
+              <a:ext cx="2914901" cy="495072"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑧</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>= </m:t>
+                    </m:r>
+                    <m:nary>
+                      <m:naryPr>
+                        <m:chr m:val="∑"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>4</m:t>
+                        </m:r>
+                      </m:sup>
+                      <m:e>
+                        <m:nary>
+                          <m:naryPr>
+                            <m:chr m:val="∑"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:naryPr>
+                          <m:sub>
+                            <m:r>
+                              <m:rPr>
+                                <m:brk m:alnAt="23"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑘</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:r>
+                              <m:rPr>
+                                <m:brk m:alnAt="23"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sup>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑐𝑖𝑘</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥𝑖𝑘</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+ </m:t>
+                            </m:r>
+                            <m:nary>
+                              <m:naryPr>
+                                <m:chr m:val="∑"/>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:naryPr>
+                              <m:sub>
+                                <m:r>
+                                  <m:rPr>
+                                    <m:brk m:alnAt="23"/>
+                                  </m:rPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑘</m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>=</m:t>
+                                </m:r>
+                                <m:r>
+                                  <m:rPr>
+                                    <m:brk m:alnAt="23"/>
+                                  </m:rPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                              </m:sub>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>3</m:t>
+                                </m:r>
+                              </m:sup>
+                              <m:e>
+                                <m:nary>
+                                  <m:naryPr>
+                                    <m:chr m:val="∑"/>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:naryPr>
+                                  <m:sub>
+                                    <m:r>
+                                      <m:rPr>
+                                        <m:brk m:alnAt="23"/>
+                                      </m:rPr>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑗</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>=</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <m:rPr>
+                                        <m:brk m:alnAt="23"/>
+                                      </m:rPr>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>1</m:t>
+                                    </m:r>
+                                  </m:sub>
+                                  <m:sup>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>3</m:t>
+                                    </m:r>
+                                  </m:sup>
+                                  <m:e>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑐𝑘𝑗</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>∗</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑥𝑘𝑗</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t> →</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑚𝑖𝑛</m:t>
+                                    </m:r>
+                                  </m:e>
+                                </m:nary>
+                              </m:e>
+                            </m:nary>
+                          </m:e>
+                        </m:nary>
+                      </m:e>
+                    </m:nary>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12233F23-6E7E-E5A4-224B-8A8A6A608589}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7305675" y="4414837"/>
+              <a:ext cx="2914901" cy="495072"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑧= ∑24_(𝑖=1)^4▒∑24_(𝑘=1)^3▒〖𝑐𝑖𝑘∗𝑥𝑖𝑘+ ∑24_(𝑘=1)^3▒∑24_(𝑗=1)^3▒〖𝑐𝑘𝑗∗𝑥𝑘𝑗 →𝑚𝑖𝑛〗〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1324850" cy="475964"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09892A27-88B3-09F5-F081-4A18F95ECA7E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7077075" y="4986337"/>
+              <a:ext cx="1324850" cy="475964"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:nary>
+                      <m:naryPr>
+                        <m:chr m:val="∑"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="ru-RU" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥𝑖𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>≤</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎𝑖</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>, </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>= </m:t>
+                        </m:r>
+                        <m:acc>
+                          <m:accPr>
+                            <m:chr m:val="̅"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:accPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>, </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>4</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:acc>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:e>
+                    </m:nary>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09892A27-88B3-09F5-F081-4A18F95ECA7E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7077075" y="4986337"/>
+              <a:ext cx="1324850" cy="475964"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑24_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑘=1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>3</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>▒〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥𝑖𝑘≤𝑎𝑖, 𝑖= (1, 4) ̅  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1380763" cy="475195"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B977AF-73B0-47D5-A40B-2102C68DA11E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7086600" y="5548312"/>
+              <a:ext cx="1380763" cy="475195"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:nary>
+                      <m:naryPr>
+                        <m:chr m:val="∑"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="ru-RU" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>4</m:t>
+                        </m:r>
+                      </m:sup>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥𝑖𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>≤</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>, </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>= </m:t>
+                        </m:r>
+                        <m:acc>
+                          <m:accPr>
+                            <m:chr m:val="̅"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:accPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>, </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:acc>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:e>
+                    </m:nary>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B977AF-73B0-47D5-A40B-2102C68DA11E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7086600" y="5548312"/>
+              <a:ext cx="1380763" cy="475195"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑24_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖=1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>▒〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥𝑖𝑘≤𝑑𝑘, 𝑘= (1, 3) ̅  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1334596" cy="475964"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC9FD66A-156C-4234-8479-1741434DAAF5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7105650" y="6129337"/>
+              <a:ext cx="1334596" cy="475964"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:nary>
+                      <m:naryPr>
+                        <m:chr m:val="∑"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="ru-RU" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥𝑘𝑗</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>≥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏𝑗</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>, </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑗</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>= </m:t>
+                        </m:r>
+                        <m:acc>
+                          <m:accPr>
+                            <m:chr m:val="̅"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:accPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>, </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:acc>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:e>
+                    </m:nary>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC9FD66A-156C-4234-8479-1741434DAAF5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7105650" y="6129337"/>
+              <a:ext cx="1334596" cy="475964"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑24_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑘=1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>3</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>▒〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥𝑘𝑗≥𝑏𝑗, 𝑗= (1, 3) ̅  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1016368" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156931DA-01A3-CDE5-DC46-36CBD6A97E99}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8972550" y="5148262"/>
+              <a:ext cx="1016368" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥𝑖𝑘</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>0</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>, </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥𝑘𝑗</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>0</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156931DA-01A3-CDE5-DC46-36CBD6A97E99}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8972550" y="5148262"/>
+              <a:ext cx="1016368" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥𝑖𝑘≥0, 𝑥𝑘𝑗≥0</a:t>
+              </a:r>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9279,7 +10684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
@@ -9290,18 +10695,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9319,9 +10724,9 @@
       <c r="E2" s="2">
         <v>2000</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
@@ -9344,9 +10749,9 @@
       <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -9367,9 +10772,9 @@
       <c r="E4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="18" t="s">
         <v>4</v>
       </c>
@@ -9392,9 +10797,9 @@
       <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
@@ -9415,17 +10820,17 @@
       <c r="E6" s="2">
         <v>9</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="21" t="s">
         <v>5</v>
       </c>
@@ -9433,29 +10838,29 @@
       <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -9478,17 +10883,17 @@
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="22"/>
-      <c r="W13" s="22"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -9509,17 +10914,17 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -9537,17 +10942,17 @@
       <c r="E15" s="2">
         <v>3</v>
       </c>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
     </row>
     <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -9565,22 +10970,22 @@
       <c r="E16" s="2">
         <v>4</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -9598,20 +11003,20 @@
       <c r="E17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -9629,230 +11034,230 @@
       <c r="E18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
-      <c r="U21" s="22"/>
-      <c r="V21" s="22"/>
-      <c r="W21" s="22"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="22"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
-      <c r="W23" s="22"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="22"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="22"/>
-      <c r="U25" s="22"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="22"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
     </row>
     <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -9870,17 +11275,17 @@
       <c r="E30" s="2">
         <v>2000</v>
       </c>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22"/>
-      <c r="U30" s="22"/>
-      <c r="V30" s="22"/>
-      <c r="W30" s="22"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
@@ -9905,17 +11310,17 @@
       <c r="I31" t="s">
         <v>18</v>
       </c>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="22"/>
-      <c r="S31" s="22"/>
-      <c r="T31" s="22"/>
-      <c r="U31" s="22"/>
-      <c r="V31" s="22"/>
-      <c r="W31" s="22"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
@@ -9939,17 +11344,17 @@
       <c r="I32" t="s">
         <v>19</v>
       </c>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="22"/>
-      <c r="V32" s="22"/>
-      <c r="W32" s="22"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
@@ -9971,21 +11376,21 @@
         <v>0</v>
       </c>
       <c r="H33" s="10"/>
-      <c r="I33" s="22" t="s">
+      <c r="I33" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="22"/>
-      <c r="U33" s="22"/>
-      <c r="V33" s="22"/>
-      <c r="W33" s="22"/>
+      <c r="J33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
@@ -10004,17 +11409,17 @@
         <v>-4</v>
       </c>
       <c r="F34" s="18"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="22"/>
-      <c r="W34" s="22"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
@@ -10035,17 +11440,17 @@
       <c r="F35" s="18">
         <v>1</v>
       </c>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
-      <c r="U35" s="22"/>
-      <c r="V35" s="22"/>
-      <c r="W35" s="22"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
     </row>
     <row r="36" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
@@ -10064,17 +11469,17 @@
         <v>-4</v>
       </c>
       <c r="F36" s="18"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="22"/>
-      <c r="U36" s="22"/>
-      <c r="V36" s="22"/>
-      <c r="W36" s="22"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
@@ -10151,7 +11556,7 @@
       <c r="E40" s="3">
         <v>1000</v>
       </c>
-      <c r="F40" s="19"/>
+      <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
@@ -10175,10 +11580,10 @@
       <c r="I41" s="2">
         <v>500</v>
       </c>
-      <c r="J41" s="17" t="s">
+      <c r="J41" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K41" s="17"/>
+      <c r="K41" s="22"/>
       <c r="L41">
         <f>D31*D32+B33*B34+C33*C34+B35*B36+D35*D36+D37*D38+E37*E38</f>
         <v>20500</v>
@@ -10394,7 +11799,7 @@
       <c r="E53" s="3">
         <v>1000</v>
       </c>
-      <c r="F53" s="19"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
@@ -10418,10 +11823,10 @@
       <c r="I54" s="2">
         <v>500</v>
       </c>
-      <c r="J54" s="17" t="s">
+      <c r="J54" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K54" s="17"/>
+      <c r="K54" s="22"/>
       <c r="L54">
         <f>D44*D45+C46*C47+B46*B47+B48*B49+E48*E49+D50*D51+E50*E51</f>
         <v>18500</v>
@@ -10638,7 +12043,7 @@
       <c r="E66" s="3">
         <v>1000</v>
       </c>
-      <c r="F66" s="19"/>
+      <c r="F66" s="23"/>
     </row>
     <row r="67" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
@@ -10662,10 +12067,10 @@
       <c r="I67" s="2">
         <v>500</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="J67" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K67" s="17"/>
+      <c r="K67" s="22"/>
       <c r="L67">
         <f>D57*D58+C59*C60+B59*B60+B61*B62+E61*E62+C63*C64+D63*D64</f>
         <v>16500</v>
@@ -10880,7 +12285,7 @@
       <c r="E79" s="3">
         <v>1000</v>
       </c>
-      <c r="F79" s="19"/>
+      <c r="F79" s="23"/>
     </row>
     <row r="80" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="2">
@@ -10898,10 +12303,10 @@
       <c r="F80" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H80" s="17" t="s">
+      <c r="H80" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I80" s="17"/>
+      <c r="I80" s="22"/>
       <c r="J80">
         <f>D70*D71+D72*D73+B72*B73+B74*B75+E74*E75+C76*C77+D76*D77</f>
         <v>16000</v>
@@ -10909,27 +12314,28 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="M13:W28"/>
-    <mergeCell ref="M30:W36"/>
-    <mergeCell ref="A22:K28"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="G4:I6"/>
-    <mergeCell ref="G7:I9"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="F63:F64"/>
     <mergeCell ref="J4:L6"/>
     <mergeCell ref="J7:L9"/>
     <mergeCell ref="J2:L3"/>
@@ -10946,28 +12352,27 @@
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="F52:F53"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="G4:I6"/>
+    <mergeCell ref="G7:I9"/>
+    <mergeCell ref="M13:W28"/>
+    <mergeCell ref="M30:W36"/>
+    <mergeCell ref="A22:K28"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="F48:F49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10985,18 +12390,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -11014,9 +12419,9 @@
       <c r="E2" s="2">
         <v>2000</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
@@ -11039,9 +12444,9 @@
       <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -11062,9 +12467,9 @@
       <c r="E4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="18" t="s">
         <v>4</v>
       </c>
@@ -11087,9 +12492,9 @@
       <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
@@ -11110,17 +12515,17 @@
       <c r="E6" s="2">
         <v>9</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="21" t="s">
         <v>5</v>
       </c>
@@ -11128,17 +12533,17 @@
       <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -11203,11 +12608,11 @@
         <v>500</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -11575,7 +12980,7 @@
         <f>F32-(F$34+$G32)</f>
         <v>2</v>
       </c>
-      <c r="G33" s="19"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
@@ -11602,10 +13007,10 @@
       <c r="J34" s="2">
         <v>0</v>
       </c>
-      <c r="K34" s="17" t="s">
+      <c r="K34" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L34" s="17"/>
+      <c r="L34" s="22"/>
       <c r="M34" s="2">
         <f>D24*D25+C26*C27+B26*B27+B28*B29+D28*D29+F28*F29+D30*D31</f>
         <v>11500</v>
@@ -11854,7 +13259,7 @@
         <f>F45-(F$47+$G45)</f>
         <v>2</v>
       </c>
-      <c r="G46" s="19"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
@@ -11881,10 +13286,10 @@
       <c r="J47" s="2">
         <v>1000</v>
       </c>
-      <c r="K47" s="17" t="s">
+      <c r="K47" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L47" s="17"/>
+      <c r="L47" s="22"/>
       <c r="M47" s="2">
         <f>D37*D38+C39*C40+D39*D40+B41*B42+D41*D42+F41*F42+D43*D44</f>
         <v>11500</v>
@@ -12135,7 +13540,7 @@
         <f>F58-(F$60+$G58)</f>
         <v>2</v>
       </c>
-      <c r="G59" s="19"/>
+      <c r="G59" s="23"/>
     </row>
     <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
@@ -12156,10 +13561,10 @@
       <c r="G60" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I60" s="17" t="s">
+      <c r="I60" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J60" s="17"/>
+      <c r="J60" s="22"/>
       <c r="K60" s="2">
         <f>D50*D51+D52*D53+B54*B55+D54*D55+F54*F55+C56*C57+D56*D57</f>
         <v>10500</v>
@@ -12334,10 +13739,10 @@
         <v>0</v>
       </c>
       <c r="F73" s="15"/>
-      <c r="G73" s="17" t="s">
+      <c r="G73" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H73" s="17"/>
+      <c r="H73" s="22"/>
       <c r="I73" s="18">
         <f>D65*D66+D67*D68+B69*B70+D69*D70+C71*C72+E71*E72</f>
         <v>19500</v>
@@ -12352,41 +13757,19 @@
         <v>1000</v>
       </c>
       <c r="F74" s="4"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
       <c r="I74" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G7:I9"/>
-    <mergeCell ref="J7:L9"/>
-    <mergeCell ref="A14:F15"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="G4:I6"/>
-    <mergeCell ref="J4:L6"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G73:H74"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A73:A74"/>
     <mergeCell ref="A62:E63"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="G58:G59"/>
@@ -12403,13 +13786,35 @@
     <mergeCell ref="G56:G57"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G73:H74"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="G7:I9"/>
+    <mergeCell ref="J7:L9"/>
+    <mergeCell ref="A14:F15"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="G4:I6"/>
+    <mergeCell ref="J4:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12427,13 +13832,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -12538,20 +13943,20 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -12686,13 +14091,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -12815,13 +14220,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -12946,10 +14351,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF048BF-D913-43C4-9BC0-F50BDDE95D42}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12958,13 +14363,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
@@ -12973,13 +14378,13 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
       <c r="Q1" s="18" t="s">
         <v>49</v>
       </c>
@@ -12989,17 +14394,15 @@
       <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="23"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>46</v>
@@ -13012,17 +14415,15 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="23"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
         <v>46</v>
@@ -13038,7 +14439,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="2">
@@ -13069,7 +14470,7 @@
         <v>220</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="2">
@@ -13104,7 +14505,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="2">
@@ -13135,7 +14536,7 @@
         <v>280</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="2">
@@ -13170,7 +14571,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="2">
@@ -13201,7 +14602,7 @@
         <v>250</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="2" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="2">
@@ -13236,7 +14637,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="2">
@@ -13263,7 +14664,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="M6" s="2">
@@ -13309,7 +14710,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="M7" s="2">
@@ -13337,15 +14738,15 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -13366,20 +14767,20 @@
       <c r="G10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="L10" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22" t="s">
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -13403,32 +14804,32 @@
       <c r="G11" s="2">
         <v>1000</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11" s="2">
         <v>3</v>
       </c>
-      <c r="M11" s="25">
-        <v>0</v>
-      </c>
-      <c r="N11" s="25">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
         <v>197</v>
       </c>
-      <c r="O11" s="25">
+      <c r="O11" s="2">
         <f>SUM(L11:N11)</f>
         <v>200</v>
       </c>
-      <c r="Q11" s="25">
-        <v>0</v>
-      </c>
-      <c r="R11" s="25">
-        <v>0</v>
-      </c>
-      <c r="S11" s="25">
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
         <v>200</v>
       </c>
-      <c r="T11" s="25">
+      <c r="T11" s="2">
         <v>20</v>
       </c>
-      <c r="U11" s="25">
+      <c r="U11" s="2">
         <f>SUM(Q11:T11)</f>
         <v>220</v>
       </c>
@@ -13455,32 +14856,32 @@
       <c r="G12" s="2">
         <v>1000</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="2">
         <v>97</v>
       </c>
-      <c r="M12" s="25">
-        <v>0</v>
-      </c>
-      <c r="N12" s="25">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
         <v>53</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="2">
         <f t="shared" ref="O12:O15" si="0">SUM(L12:N12)</f>
         <v>150</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="2">
         <v>100</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="2">
         <v>150</v>
       </c>
-      <c r="S12" s="25">
-        <v>0</v>
-      </c>
-      <c r="T12" s="25">
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
         <v>30</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12" s="2">
         <f t="shared" ref="U12:U13" si="1">SUM(Q12:T12)</f>
         <v>280</v>
       </c>
@@ -13507,32 +14908,32 @@
       <c r="G13" s="2">
         <v>1000</v>
       </c>
-      <c r="L13" s="25">
-        <v>0</v>
-      </c>
-      <c r="M13" s="25">
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
         <v>100</v>
       </c>
-      <c r="N13" s="25">
-        <v>0</v>
-      </c>
-      <c r="O13" s="25">
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="2">
         <v>250</v>
       </c>
-      <c r="R13" s="25">
-        <v>0</v>
-      </c>
-      <c r="S13" s="25">
-        <v>0</v>
-      </c>
-      <c r="T13" s="25">
-        <v>0</v>
-      </c>
-      <c r="U13" s="25">
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
@@ -13559,36 +14960,36 @@
       <c r="G14" s="2">
         <v>1000</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="2">
         <v>120</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="2">
         <v>130</v>
       </c>
-      <c r="N14" s="25">
-        <v>0</v>
-      </c>
-      <c r="O14" s="25">
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="2">
         <f>SUM(Q11:Q13)</f>
         <v>350</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="2">
         <f t="shared" ref="R14:T14" si="2">SUM(R11:R13)</f>
         <v>150</v>
       </c>
-      <c r="S14" s="25">
+      <c r="S14" s="2">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="T14" s="25">
+      <c r="T14" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="U14" s="26">
+      <c r="U14" s="17">
         <f>SUMPRODUCT(R3:U5,Q11:T13)</f>
         <v>8700</v>
       </c>
@@ -13615,16 +15016,16 @@
       <c r="G15" s="2">
         <v>16</v>
       </c>
-      <c r="L15" s="25">
-        <v>0</v>
-      </c>
-      <c r="M15" s="25">
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
         <v>50</v>
       </c>
-      <c r="N15" s="25">
-        <v>0</v>
-      </c>
-      <c r="O15" s="25">
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -13651,26 +15052,26 @@
       <c r="G16" s="2">
         <v>24</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="2">
         <f>SUM(L11:L15)</f>
         <v>220</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="2">
         <f t="shared" ref="M16:N16" si="3">SUM(M11:M15)</f>
         <v>280</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="2">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="O16" s="26">
+      <c r="O16" s="17">
         <f>SUMPRODUCT(M3:O7,L11:N15)</f>
         <v>2100</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="R16" s="26">
+      <c r="R16" s="17">
         <f>O16+U14</f>
         <v>10800</v>
       </c>
@@ -13713,15 +15114,15 @@
       <c r="U18" s="18"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
@@ -13816,6 +15217,14 @@
       <c r="I22" s="2">
         <v>150</v>
       </c>
+      <c r="L22" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -13846,6 +15255,12 @@
       <c r="I23" s="2">
         <v>100</v>
       </c>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -13876,6 +15291,12 @@
       <c r="I24" s="2">
         <v>250</v>
       </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -13906,6 +15327,12 @@
       <c r="I25" s="2">
         <v>220</v>
       </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -13936,6 +15363,12 @@
       <c r="I26" s="2">
         <v>280</v>
       </c>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -13966,6 +15399,12 @@
       <c r="I27" s="2">
         <v>250</v>
       </c>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -13992,6 +15431,12 @@
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -14016,10 +15461,21 @@
       <c r="G29" s="2">
         <v>200</v>
       </c>
-      <c r="I29" s="26">
+      <c r="I29" s="17">
         <f>SUMPRODUCT(B11:G17,B21:G27)</f>
         <v>10800</v>
       </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
@@ -14033,9 +15489,9 @@
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
@@ -14053,9 +15509,9 @@
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
@@ -14063,20 +15519,42 @@
       <c r="S32" s="12"/>
       <c r="T32" s="12"/>
     </row>
+    <row r="33" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+    </row>
+    <row r="34" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+    </row>
+    <row r="35" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
+    <mergeCell ref="L33:N35"/>
+    <mergeCell ref="O27:Q29"/>
+    <mergeCell ref="L22:Q23"/>
+    <mergeCell ref="L24:Q26"/>
+    <mergeCell ref="L27:N29"/>
+    <mergeCell ref="L30:N32"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A31:I32"/>
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="L10:P10"/>
     <mergeCell ref="Q10:U10"/>
     <mergeCell ref="L18:U19"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A31:I32"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>